<commit_message>
- added utils functions + gitignore
</commit_message>
<xml_diff>
--- a/data/fitness_stats.xlsx
+++ b/data/fitness_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fedrigonigroup-my.sharepoint.com/personal/matteo_stori_fedrigoni_com/Documents/Documents/99. Workspaces/eclipse-workspace/fitness_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2991" documentId="13_ncr:1_{B553671A-B275-47B2-9845-BC0F12C1290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20CA65B5-8722-4B51-8CAA-05301BB87193}"/>
+  <xr:revisionPtr revIDLastSave="2995" documentId="13_ncr:1_{B553671A-B275-47B2-9845-BC0F12C1290D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{022FF1D1-5F79-4D2D-B213-E112C71C6E07}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B7E11E8D-C27E-458E-A60B-3A037DE09D8F}"/>
   </bookViews>
@@ -543,7 +543,7 @@
     <t>Biceps sets</t>
   </si>
   <si>
-    <t>Core sets2</t>
+    <t>Core kg</t>
   </si>
 </sst>
 </file>
@@ -931,13 +931,13 @@
     <tableColumn id="13" xr3:uid="{5F767AC0-B91D-4EDB-B67B-529FDC357076}" name="Back kg" dataDxfId="13"/>
     <tableColumn id="14" xr3:uid="{7FC1A188-A6B5-4578-9B58-F1FFDE047003}" name="Shoulders kg" dataDxfId="12"/>
     <tableColumn id="15" xr3:uid="{DA59A4B0-924A-463F-B080-F79CC400B465}" name="Biceps kg" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{8F1CC787-1469-4B9B-8777-20FA923D65BF}" name="Core sets" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{8F1CC787-1469-4B9B-8777-20FA923D65BF}" name="Core kg" dataDxfId="10"/>
     <tableColumn id="17" xr3:uid="{8D7AD44F-F7EC-49D1-8117-7B2006D00941}" name="Leg sets" dataDxfId="9"/>
     <tableColumn id="18" xr3:uid="{76C118E7-C404-4800-B5CF-CF6F93948E3D}" name="Chest sets" dataDxfId="8"/>
     <tableColumn id="19" xr3:uid="{7BB3BE0E-4E0A-470F-870A-E23B14532532}" name="Back sets" dataDxfId="7"/>
     <tableColumn id="20" xr3:uid="{D70AFB19-6ABB-4C9C-ACB5-5DC0C3BB3465}" name="Shoulders sets" dataDxfId="6"/>
     <tableColumn id="21" xr3:uid="{DCAB7665-3442-4657-94FA-96414BDB7797}" name="Biceps sets" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{32ABDA74-77BB-4223-995D-2D6A0E436F2F}" name="Core sets2" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{32ABDA74-77BB-4223-995D-2D6A0E436F2F}" name="Core sets" dataDxfId="4"/>
     <tableColumn id="23" xr3:uid="{9DC50228-6B28-4087-BFA7-CB58CEE42BB1}" name="Mins run" dataDxfId="3">
       <calculatedColumnFormula>SUMIF(#REF!,'Weekly Calendar summary'!$C2,#REF!)</calculatedColumnFormula>
     </tableColumn>
@@ -3473,8 +3473,8 @@
   <dimension ref="A1:AC127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3552,7 +3552,7 @@
         <v>160</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>162</v>
@@ -3570,7 +3570,7 @@
         <v>166</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="Y1" s="7" t="s">
         <v>71</v>
@@ -3625,7 +3625,9 @@
       <c r="Q2" s="9">
         <v>0</v>
       </c>
-      <c r="R2" s="11"/>
+      <c r="R2" s="11">
+        <v>0</v>
+      </c>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
       <c r="U2" s="11"/>
@@ -3686,7 +3688,9 @@
       <c r="Q3" s="9">
         <v>0</v>
       </c>
-      <c r="R3" s="11"/>
+      <c r="R3" s="11">
+        <v>0</v>
+      </c>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
       <c r="U3" s="11"/>
@@ -3747,7 +3751,9 @@
       <c r="Q4" s="9">
         <v>0</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="11">
+        <v>0</v>
+      </c>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="11"/>
@@ -3808,7 +3814,9 @@
       <c r="Q5" s="9">
         <v>1000</v>
       </c>
-      <c r="R5" s="11"/>
+      <c r="R5" s="11">
+        <v>0</v>
+      </c>
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
       <c r="U5" s="11"/>
@@ -3869,7 +3877,9 @@
       <c r="Q6" s="9">
         <v>256</v>
       </c>
-      <c r="R6" s="11"/>
+      <c r="R6" s="11">
+        <v>0</v>
+      </c>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="11"/>
@@ -3930,7 +3940,9 @@
       <c r="Q7" s="9">
         <v>300</v>
       </c>
-      <c r="R7" s="11"/>
+      <c r="R7" s="11">
+        <v>0</v>
+      </c>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="11"/>
@@ -3991,7 +4003,9 @@
       <c r="Q8" s="9">
         <v>960</v>
       </c>
-      <c r="R8" s="11"/>
+      <c r="R8" s="11">
+        <v>0</v>
+      </c>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
       <c r="U8" s="11"/>
@@ -4052,7 +4066,9 @@
       <c r="Q9" s="9">
         <v>640</v>
       </c>
-      <c r="R9" s="11"/>
+      <c r="R9" s="11">
+        <v>0</v>
+      </c>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="11"/>
@@ -4113,7 +4129,9 @@
       <c r="Q10" s="9">
         <v>768</v>
       </c>
-      <c r="R10" s="11"/>
+      <c r="R10" s="11">
+        <v>0</v>
+      </c>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="11"/>
@@ -4174,7 +4192,9 @@
       <c r="Q11" s="9">
         <v>768</v>
       </c>
-      <c r="R11" s="11"/>
+      <c r="R11" s="11">
+        <v>0</v>
+      </c>
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="11"/>
@@ -4235,7 +4255,9 @@
       <c r="Q12" s="9">
         <v>745.6</v>
       </c>
-      <c r="R12" s="11"/>
+      <c r="R12" s="11">
+        <v>0</v>
+      </c>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="11"/>
@@ -4296,7 +4318,9 @@
       <c r="Q13" s="9">
         <v>0</v>
       </c>
-      <c r="R13" s="11"/>
+      <c r="R13" s="11">
+        <v>0</v>
+      </c>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="11"/>
@@ -4357,7 +4381,9 @@
       <c r="Q14" s="9">
         <v>0</v>
       </c>
-      <c r="R14" s="11"/>
+      <c r="R14" s="11">
+        <v>0</v>
+      </c>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="11"/>
@@ -4418,7 +4444,9 @@
       <c r="Q15" s="9">
         <v>480</v>
       </c>
-      <c r="R15" s="11"/>
+      <c r="R15" s="11">
+        <v>0</v>
+      </c>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="11"/>
@@ -4479,7 +4507,9 @@
       <c r="Q16" s="9">
         <v>0</v>
       </c>
-      <c r="R16" s="11"/>
+      <c r="R16" s="11">
+        <v>0</v>
+      </c>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="11"/>
@@ -4540,7 +4570,9 @@
       <c r="Q17" s="9">
         <v>384</v>
       </c>
-      <c r="R17" s="11"/>
+      <c r="R17" s="11">
+        <v>0</v>
+      </c>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="11"/>
@@ -4601,7 +4633,9 @@
       <c r="Q18" s="9">
         <v>640</v>
       </c>
-      <c r="R18" s="11"/>
+      <c r="R18" s="11">
+        <v>0</v>
+      </c>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="U18" s="11"/>
@@ -4662,7 +4696,9 @@
       <c r="Q19" s="9">
         <v>0</v>
       </c>
-      <c r="R19" s="11"/>
+      <c r="R19" s="11">
+        <v>0</v>
+      </c>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
       <c r="U19" s="11"/>
@@ -4723,7 +4759,9 @@
       <c r="Q20" s="9">
         <v>0</v>
       </c>
-      <c r="R20" s="11"/>
+      <c r="R20" s="11">
+        <v>0</v>
+      </c>
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="11"/>
@@ -4784,7 +4822,9 @@
       <c r="Q21" s="9">
         <v>0</v>
       </c>
-      <c r="R21" s="11"/>
+      <c r="R21" s="11">
+        <v>0</v>
+      </c>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
       <c r="U21" s="11"/>
@@ -4845,7 +4885,9 @@
       <c r="Q22" s="9">
         <v>0</v>
       </c>
-      <c r="R22" s="11"/>
+      <c r="R22" s="11">
+        <v>0</v>
+      </c>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
       <c r="U22" s="11"/>
@@ -4908,7 +4950,9 @@
       <c r="Q23" s="9">
         <v>0</v>
       </c>
-      <c r="R23" s="11"/>
+      <c r="R23" s="11">
+        <v>0</v>
+      </c>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
       <c r="U23" s="11"/>
@@ -4975,7 +5019,9 @@
       <c r="Q24" s="9">
         <v>0</v>
       </c>
-      <c r="R24" s="11"/>
+      <c r="R24" s="11">
+        <v>0</v>
+      </c>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="U24" s="11"/>
@@ -5042,7 +5088,9 @@
       <c r="Q25" s="9">
         <v>864</v>
       </c>
-      <c r="R25" s="11"/>
+      <c r="R25" s="11">
+        <v>0</v>
+      </c>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="11"/>
@@ -5109,7 +5157,9 @@
       <c r="Q26" s="9">
         <v>0</v>
       </c>
-      <c r="R26" s="11"/>
+      <c r="R26" s="11">
+        <v>0</v>
+      </c>
       <c r="S26" s="12"/>
       <c r="T26" s="12"/>
       <c r="U26" s="11"/>
@@ -5176,7 +5226,9 @@
       <c r="Q27" s="9">
         <v>0</v>
       </c>
-      <c r="R27" s="11"/>
+      <c r="R27" s="11">
+        <v>0</v>
+      </c>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
       <c r="U27" s="11"/>
@@ -5243,7 +5295,9 @@
       <c r="Q28" s="9">
         <v>0</v>
       </c>
-      <c r="R28" s="11"/>
+      <c r="R28" s="11">
+        <v>0</v>
+      </c>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="11"/>
@@ -5310,7 +5364,9 @@
       <c r="Q29" s="9">
         <v>0</v>
       </c>
-      <c r="R29" s="11"/>
+      <c r="R29" s="11">
+        <v>0</v>
+      </c>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
       <c r="U29" s="11"/>
@@ -5377,7 +5433,9 @@
       <c r="Q30" s="9">
         <v>0</v>
       </c>
-      <c r="R30" s="11"/>
+      <c r="R30" s="11">
+        <v>0</v>
+      </c>
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="U30" s="11"/>
@@ -5448,7 +5506,9 @@
       <c r="Q31" s="9">
         <v>960</v>
       </c>
-      <c r="R31" s="11"/>
+      <c r="R31" s="11">
+        <v>0</v>
+      </c>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="11"/>
@@ -5519,7 +5579,9 @@
       <c r="Q32" s="9">
         <v>1320</v>
       </c>
-      <c r="R32" s="11"/>
+      <c r="R32" s="11">
+        <v>0</v>
+      </c>
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
       <c r="U32" s="11"/>
@@ -5590,7 +5652,9 @@
       <c r="Q33" s="9">
         <v>2760</v>
       </c>
-      <c r="R33" s="11"/>
+      <c r="R33" s="11">
+        <v>0</v>
+      </c>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="11"/>
@@ -5661,7 +5725,9 @@
       <c r="Q34" s="9">
         <v>1000</v>
       </c>
-      <c r="R34" s="11"/>
+      <c r="R34" s="11">
+        <v>0</v>
+      </c>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="11"/>
@@ -5732,7 +5798,9 @@
       <c r="Q35" s="9">
         <v>2400</v>
       </c>
-      <c r="R35" s="11"/>
+      <c r="R35" s="11">
+        <v>0</v>
+      </c>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
       <c r="U35" s="11"/>
@@ -5803,7 +5871,9 @@
       <c r="Q36" s="9">
         <v>2736</v>
       </c>
-      <c r="R36" s="11"/>
+      <c r="R36" s="11">
+        <v>0</v>
+      </c>
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
       <c r="U36" s="11"/>
@@ -5874,7 +5944,9 @@
       <c r="Q37" s="9">
         <v>2601.6</v>
       </c>
-      <c r="R37" s="11"/>
+      <c r="R37" s="11">
+        <v>0</v>
+      </c>
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="11"/>
@@ -5945,7 +6017,9 @@
       <c r="Q38" s="9">
         <v>1640</v>
       </c>
-      <c r="R38" s="11"/>
+      <c r="R38" s="11">
+        <v>0</v>
+      </c>
       <c r="S38" s="12"/>
       <c r="T38" s="12"/>
       <c r="U38" s="11"/>
@@ -6016,7 +6090,9 @@
       <c r="Q39" s="9">
         <v>2320</v>
       </c>
-      <c r="R39" s="11"/>
+      <c r="R39" s="11">
+        <v>0</v>
+      </c>
       <c r="S39" s="12"/>
       <c r="T39" s="12"/>
       <c r="U39" s="11"/>
@@ -6087,7 +6163,9 @@
       <c r="Q40" s="9">
         <v>1920</v>
       </c>
-      <c r="R40" s="11"/>
+      <c r="R40" s="11">
+        <v>0</v>
+      </c>
       <c r="S40" s="12"/>
       <c r="T40" s="12"/>
       <c r="U40" s="11"/>
@@ -6158,7 +6236,9 @@
       <c r="Q41" s="9">
         <v>3200</v>
       </c>
-      <c r="R41" s="11"/>
+      <c r="R41" s="11">
+        <v>0</v>
+      </c>
       <c r="S41" s="12"/>
       <c r="T41" s="12"/>
       <c r="U41" s="11"/>
@@ -6229,7 +6309,9 @@
       <c r="Q42" s="9">
         <v>320</v>
       </c>
-      <c r="R42" s="11"/>
+      <c r="R42" s="11">
+        <v>0</v>
+      </c>
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="11"/>
@@ -6300,7 +6382,9 @@
       <c r="Q43" s="9">
         <v>3360</v>
       </c>
-      <c r="R43" s="11"/>
+      <c r="R43" s="11">
+        <v>0</v>
+      </c>
       <c r="S43" s="12"/>
       <c r="T43" s="12"/>
       <c r="U43" s="11"/>
@@ -6371,7 +6455,9 @@
       <c r="Q44" s="9">
         <v>723.2</v>
       </c>
-      <c r="R44" s="11"/>
+      <c r="R44" s="11">
+        <v>0</v>
+      </c>
       <c r="S44" s="12"/>
       <c r="T44" s="12"/>
       <c r="U44" s="11"/>
@@ -6442,7 +6528,9 @@
       <c r="Q45" s="9">
         <v>761.59999999999991</v>
       </c>
-      <c r="R45" s="11"/>
+      <c r="R45" s="11">
+        <v>0</v>
+      </c>
       <c r="S45" s="12"/>
       <c r="T45" s="12"/>
       <c r="U45" s="11"/>
@@ -6513,7 +6601,9 @@
       <c r="Q46" s="9">
         <v>2265.6</v>
       </c>
-      <c r="R46" s="11"/>
+      <c r="R46" s="11">
+        <v>0</v>
+      </c>
       <c r="S46" s="12"/>
       <c r="T46" s="12"/>
       <c r="U46" s="11"/>
@@ -6584,7 +6674,9 @@
       <c r="Q47" s="9">
         <v>3440</v>
       </c>
-      <c r="R47" s="11"/>
+      <c r="R47" s="11">
+        <v>0</v>
+      </c>
       <c r="S47" s="12"/>
       <c r="T47" s="12"/>
       <c r="U47" s="11"/>
@@ -6655,7 +6747,9 @@
       <c r="Q48" s="9">
         <v>1680</v>
       </c>
-      <c r="R48" s="11"/>
+      <c r="R48" s="11">
+        <v>0</v>
+      </c>
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="11"/>
@@ -6726,7 +6820,9 @@
       <c r="Q49" s="9">
         <v>2041.1000000000001</v>
       </c>
-      <c r="R49" s="11"/>
+      <c r="R49" s="11">
+        <v>0</v>
+      </c>
       <c r="S49" s="12"/>
       <c r="T49" s="12"/>
       <c r="U49" s="11"/>
@@ -6797,7 +6893,9 @@
       <c r="Q50" s="9">
         <v>2820.3</v>
       </c>
-      <c r="R50" s="11"/>
+      <c r="R50" s="11">
+        <v>0</v>
+      </c>
       <c r="S50" s="12"/>
       <c r="T50" s="12"/>
       <c r="U50" s="11"/>
@@ -6868,7 +6966,9 @@
       <c r="Q51" s="9">
         <v>840</v>
       </c>
-      <c r="R51" s="11"/>
+      <c r="R51" s="11">
+        <v>0</v>
+      </c>
       <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="11"/>
@@ -6939,7 +7039,9 @@
       <c r="Q52" s="9">
         <v>2960</v>
       </c>
-      <c r="R52" s="11"/>
+      <c r="R52" s="11">
+        <v>0</v>
+      </c>
       <c r="S52" s="12"/>
       <c r="T52" s="12"/>
       <c r="U52" s="11"/>
@@ -7010,7 +7112,9 @@
       <c r="Q53" s="9">
         <v>3245</v>
       </c>
-      <c r="R53" s="11"/>
+      <c r="R53" s="11">
+        <v>0</v>
+      </c>
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
       <c r="U53" s="11"/>
@@ -7081,7 +7185,9 @@
       <c r="Q54" s="9">
         <v>3420</v>
       </c>
-      <c r="R54" s="11"/>
+      <c r="R54" s="11">
+        <v>0</v>
+      </c>
       <c r="S54" s="12"/>
       <c r="T54" s="12"/>
       <c r="U54" s="11"/>
@@ -7152,7 +7258,9 @@
       <c r="Q55" s="9">
         <v>2320</v>
       </c>
-      <c r="R55" s="11"/>
+      <c r="R55" s="11">
+        <v>0</v>
+      </c>
       <c r="S55" s="12"/>
       <c r="T55" s="12"/>
       <c r="U55" s="11"/>
@@ -7223,7 +7331,9 @@
       <c r="Q56" s="9">
         <v>4260</v>
       </c>
-      <c r="R56" s="11"/>
+      <c r="R56" s="11">
+        <v>0</v>
+      </c>
       <c r="S56" s="12"/>
       <c r="T56" s="12"/>
       <c r="U56" s="11"/>
@@ -7294,7 +7404,9 @@
       <c r="Q57" s="9">
         <v>2176</v>
       </c>
-      <c r="R57" s="11"/>
+      <c r="R57" s="11">
+        <v>0</v>
+      </c>
       <c r="S57" s="12"/>
       <c r="T57" s="12"/>
       <c r="U57" s="11"/>
@@ -7365,7 +7477,9 @@
       <c r="Q58" s="9">
         <v>1740.8</v>
       </c>
-      <c r="R58" s="11"/>
+      <c r="R58" s="11">
+        <v>0</v>
+      </c>
       <c r="S58" s="12"/>
       <c r="T58" s="12"/>
       <c r="U58" s="11"/>
@@ -7436,7 +7550,9 @@
       <c r="Q59" s="9">
         <v>3140</v>
       </c>
-      <c r="R59" s="11"/>
+      <c r="R59" s="11">
+        <v>0</v>
+      </c>
       <c r="S59" s="12"/>
       <c r="T59" s="12"/>
       <c r="U59" s="11"/>
@@ -7507,7 +7623,9 @@
       <c r="Q60" s="9">
         <v>2920</v>
       </c>
-      <c r="R60" s="11"/>
+      <c r="R60" s="11">
+        <v>0</v>
+      </c>
       <c r="S60" s="12"/>
       <c r="T60" s="12"/>
       <c r="U60" s="11"/>
@@ -7578,7 +7696,9 @@
       <c r="Q61" s="9">
         <v>800</v>
       </c>
-      <c r="R61" s="11"/>
+      <c r="R61" s="11">
+        <v>0</v>
+      </c>
       <c r="S61" s="12"/>
       <c r="T61" s="12"/>
       <c r="U61" s="11"/>
@@ -7649,7 +7769,9 @@
       <c r="Q62" s="9">
         <v>900</v>
       </c>
-      <c r="R62" s="11"/>
+      <c r="R62" s="11">
+        <v>0</v>
+      </c>
       <c r="S62" s="12"/>
       <c r="T62" s="12"/>
       <c r="U62" s="11"/>
@@ -7720,7 +7842,9 @@
       <c r="Q63" s="9">
         <v>2160</v>
       </c>
-      <c r="R63" s="11"/>
+      <c r="R63" s="11">
+        <v>0</v>
+      </c>
       <c r="S63" s="12"/>
       <c r="T63" s="12"/>
       <c r="U63" s="11"/>
@@ -7791,7 +7915,9 @@
       <c r="Q64" s="9">
         <v>2880</v>
       </c>
-      <c r="R64" s="11"/>
+      <c r="R64" s="11">
+        <v>0</v>
+      </c>
       <c r="S64" s="12"/>
       <c r="T64" s="12"/>
       <c r="U64" s="11"/>
@@ -7862,7 +7988,9 @@
       <c r="Q65" s="9">
         <v>2217.6</v>
       </c>
-      <c r="R65" s="11"/>
+      <c r="R65" s="11">
+        <v>0</v>
+      </c>
       <c r="S65" s="12"/>
       <c r="T65" s="12"/>
       <c r="U65" s="11"/>
@@ -7933,7 +8061,9 @@
       <c r="Q66" s="9">
         <v>2100</v>
       </c>
-      <c r="R66" s="11"/>
+      <c r="R66" s="11">
+        <v>0</v>
+      </c>
       <c r="S66" s="12"/>
       <c r="T66" s="12"/>
       <c r="U66" s="11"/>
@@ -8004,7 +8134,9 @@
       <c r="Q67" s="9">
         <v>2100</v>
       </c>
-      <c r="R67" s="11"/>
+      <c r="R67" s="11">
+        <v>0</v>
+      </c>
       <c r="S67" s="12"/>
       <c r="T67" s="12"/>
       <c r="U67" s="11"/>
@@ -8075,7 +8207,9 @@
       <c r="Q68" s="9">
         <v>1514</v>
       </c>
-      <c r="R68" s="11"/>
+      <c r="R68" s="11">
+        <v>0</v>
+      </c>
       <c r="S68" s="12"/>
       <c r="T68" s="12"/>
       <c r="U68" s="11"/>
@@ -8146,7 +8280,9 @@
       <c r="Q69" s="9">
         <v>0</v>
       </c>
-      <c r="R69" s="11"/>
+      <c r="R69" s="11">
+        <v>0</v>
+      </c>
       <c r="S69" s="12"/>
       <c r="T69" s="12"/>
       <c r="U69" s="11"/>
@@ -8217,7 +8353,9 @@
       <c r="Q70" s="9">
         <v>2880</v>
       </c>
-      <c r="R70" s="11"/>
+      <c r="R70" s="11">
+        <v>0</v>
+      </c>
       <c r="S70" s="12"/>
       <c r="T70" s="12"/>
       <c r="U70" s="11"/>
@@ -8288,7 +8426,9 @@
       <c r="Q71" s="9">
         <v>1800</v>
       </c>
-      <c r="R71" s="11"/>
+      <c r="R71" s="11">
+        <v>0</v>
+      </c>
       <c r="S71" s="12"/>
       <c r="T71" s="12"/>
       <c r="U71" s="11"/>
@@ -8359,7 +8499,9 @@
       <c r="Q72" s="9">
         <v>720</v>
       </c>
-      <c r="R72" s="11"/>
+      <c r="R72" s="11">
+        <v>0</v>
+      </c>
       <c r="S72" s="12"/>
       <c r="T72" s="12"/>
       <c r="U72" s="11"/>
@@ -8430,7 +8572,9 @@
       <c r="Q73" s="9">
         <v>1080</v>
       </c>
-      <c r="R73" s="11"/>
+      <c r="R73" s="11">
+        <v>0</v>
+      </c>
       <c r="S73" s="12"/>
       <c r="T73" s="12"/>
       <c r="U73" s="11"/>
@@ -8501,7 +8645,9 @@
       <c r="Q74" s="9">
         <v>0</v>
       </c>
-      <c r="R74" s="11"/>
+      <c r="R74" s="11">
+        <v>0</v>
+      </c>
       <c r="S74" s="12"/>
       <c r="T74" s="12"/>
       <c r="U74" s="11"/>
@@ -8572,7 +8718,9 @@
       <c r="Q75" s="9">
         <v>0</v>
       </c>
-      <c r="R75" s="11"/>
+      <c r="R75" s="11">
+        <v>0</v>
+      </c>
       <c r="S75" s="12"/>
       <c r="T75" s="12"/>
       <c r="U75" s="11"/>

</xml_diff>